<commit_message>
Tabella Statistical analysis aggiornata con i p values
</commit_message>
<xml_diff>
--- a/Statistical_Analysis_Results.xlsx
+++ b/Statistical_Analysis_Results.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fmfm3\OneDrive\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fmfm3\OneDrive\Documenti\Git\Projectpython\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E5EB269-7DB3-40FC-910B-8F1FB8C542D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87596D33-EAF9-4F3E-9FD9-34B496E0184C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="9510" yWindow="0" windowWidth="9780" windowHeight="10170" xr2:uid="{20B7BAE8-F8E6-47E3-B5ED-62C18A4AA6AE}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="48">
   <si>
     <t>marital</t>
   </si>
@@ -267,6 +267,12 @@
   </si>
   <si>
     <t>gender</t>
+  </si>
+  <si>
+    <t>0.015</t>
+  </si>
+  <si>
+    <t>&lt;0.001</t>
   </si>
 </sst>
 </file>
@@ -667,8 +673,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E13C07C4-05E9-4C69-A2D0-D9A6ACB25012}">
   <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -706,7 +712,9 @@
       <c r="D2" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="E2" s="5"/>
+      <c r="E2" s="4" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="3" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
@@ -721,6 +729,9 @@
       <c r="D3" s="1" t="s">
         <v>44</v>
       </c>
+      <c r="E3" s="1" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="4" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
@@ -735,6 +746,9 @@
       <c r="D4" s="1" t="s">
         <v>28</v>
       </c>
+      <c r="E4" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
@@ -749,6 +763,9 @@
       <c r="D5" s="1" t="s">
         <v>30</v>
       </c>
+      <c r="E5" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
@@ -763,6 +780,9 @@
       <c r="D6" s="1" t="s">
         <v>32</v>
       </c>
+      <c r="E6" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
@@ -777,6 +797,9 @@
       <c r="D7" s="1" t="s">
         <v>34</v>
       </c>
+      <c r="E7" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
@@ -791,6 +814,9 @@
       <c r="D8" s="1" t="s">
         <v>36</v>
       </c>
+      <c r="E8" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
@@ -805,6 +831,9 @@
       <c r="D9" s="1" t="s">
         <v>38</v>
       </c>
+      <c r="E9" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
@@ -819,6 +848,9 @@
       <c r="D10" s="1" t="s">
         <v>40</v>
       </c>
+      <c r="E10" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" s="3" t="s">
@@ -832,6 +864,9 @@
       </c>
       <c r="D11" s="1" t="s">
         <v>42</v>
+      </c>
+      <c r="E11" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
@@ -851,6 +886,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101009E16C01B75DD5847899E2A379D5475FF" ma:contentTypeVersion="9" ma:contentTypeDescription="Creare un nuovo documento." ma:contentTypeScope="" ma:versionID="6f7af5ad53906506caa12eb0e3c8e977">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="2ba6efdb-b225-443d-9b4b-8c8103485182" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="058ac1251fdac5162363238a7befe9cf" ns3:_="">
     <xsd:import namespace="2ba6efdb-b225-443d-9b4b-8c8103485182"/>
@@ -1026,15 +1070,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -1044,6 +1079,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{03422A0D-02E7-4C4C-B1BA-7B29D84EB873}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F0DFFF0B-97B2-4298-898B-4BFCE0242EB9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1057,14 +1100,6 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{03422A0D-02E7-4C4C-B1BA-7B29D84EB873}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>